<commit_message>
Updating with the end of Survey Mode whistlers
Finalized the digitization of Survey Mode whistlers, and have now moved on to burst mode whistlers.
</commit_message>
<xml_diff>
--- a/Whistler_Events.xlsx
+++ b/Whistler_Events.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Desktop\GitHub\Whistler-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D36A601D-8CAE-4A9E-8540-977B3692FBBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CB3BC1-518C-481B-B83F-AFFAC3244BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6465" yWindow="4470" windowWidth="21600" windowHeight="11385" xr2:uid="{8EBB5DD4-DB68-40F9-ADC3-0C147379E945}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8EBB5DD4-DB68-40F9-ADC3-0C147379E945}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
   <si>
     <t>PJ</t>
   </si>
@@ -146,6 +147,21 @@
   </si>
   <si>
     <t>Status Burst</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Come Back To</t>
+  </si>
+  <si>
+    <t>Done, most weak signal</t>
+  </si>
+  <si>
+    <t>weak+D6:J6, hiss</t>
+  </si>
+  <si>
+    <t>None, Looks like burst will be populated</t>
   </si>
 </sst>
 </file>
@@ -207,9 +223,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -247,7 +263,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -353,7 +369,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -495,7 +511,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -506,17 +522,17 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="8.85546875" style="1"/>
-    <col min="10" max="10" width="57.7109375" customWidth="1"/>
+    <col min="1" max="9" width="8.88671875" style="1"/>
+    <col min="10" max="10" width="57.6640625" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,7 +570,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B2" s="1">
         <v>2017</v>
       </c>
@@ -582,8 +598,11 @@
       <c r="J2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
         <v>2019</v>
       </c>
@@ -609,7 +628,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>2019</v>
       </c>
@@ -637,8 +656,11 @@
       <c r="J4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>2020</v>
       </c>
@@ -666,8 +688,11 @@
       <c r="J5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>2020</v>
       </c>
@@ -693,10 +718,13 @@
         <v>6.1</v>
       </c>
       <c r="J6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="K6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>2020</v>
       </c>
@@ -724,8 +752,11 @@
       <c r="J7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>2020</v>
       </c>
@@ -753,8 +784,11 @@
       <c r="J8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>2020</v>
       </c>
@@ -782,8 +816,11 @@
       <c r="J9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>2020</v>
       </c>
@@ -811,8 +848,11 @@
       <c r="J10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -844,10 +884,10 @@
         <v>21</v>
       </c>
       <c r="K11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -875,8 +915,11 @@
       <c r="J12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -911,7 +954,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -942,8 +985,11 @@
       <c r="J14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -974,8 +1020,11 @@
       <c r="J15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -1006,8 +1055,11 @@
       <c r="J16" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>2021</v>
       </c>
@@ -1035,8 +1087,11 @@
       <c r="J17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
         <v>2021</v>
       </c>
@@ -1064,8 +1119,11 @@
       <c r="J18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
@@ -1096,8 +1154,11 @@
       <c r="J19" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
@@ -1127,6 +1188,9 @@
       </c>
       <c r="J20" t="s">
         <v>33</v>
+      </c>
+      <c r="K20" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating with first Burst
Added my progress on Burst Mode whistlers. Lots found and digitized
</commit_message>
<xml_diff>
--- a/Whistler_Events.xlsx
+++ b/Whistler_Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Desktop\GitHub\Whistler-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EB4045-88CF-4F70-AEE9-8CC4B2CFCBC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D07CC94-327C-4DA1-949D-D5E654854636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8EBB5DD4-DB68-40F9-ADC3-0C147379E945}"/>
   </bookViews>
@@ -537,7 +537,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Merging with all the new GitLab scripts and such
Adding all Autoplot scripts, resources, and cleaning out old files.
</commit_message>
<xml_diff>
--- a/Whistler_Events.xlsx
+++ b/Whistler_Events.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Desktop\GitHub\Whistler-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FB2D18-45EC-47E1-80A1-8E5F29030D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA5EEE5-C1E2-4ABC-9C81-84B95E879623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8EBB5DD4-DB68-40F9-ADC3-0C147379E945}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="63">
   <si>
     <t>PJ</t>
   </si>
@@ -157,9 +157,6 @@
     <t>No Data</t>
   </si>
   <si>
-    <t>Search through all with 2 minute axis to search for Long D</t>
-  </si>
-  <si>
     <t>Did up to 22:50, not much but rapids</t>
   </si>
   <si>
@@ -184,23 +181,68 @@
     <t>It looks like there's rapids at 17:30</t>
   </si>
   <si>
-    <t>I've also gone through survey mode and verified that the whistlers exist, and are reasonable accurate in their dispersion constant</t>
-  </si>
-  <si>
     <t>Look Earlier than Previous</t>
+  </si>
+  <si>
+    <t>To 12:41. Mediums mostly in E, but m=10 so might not be Io</t>
+  </si>
+  <si>
+    <t>To 18:09. Mediums mostly in E</t>
+  </si>
+  <si>
+    <t>To 24:00. Mediums, mostly E, sporadic across time in Burst</t>
+  </si>
+  <si>
+    <t>To 8:40. Mediums, low contrast so just do ones I'm confidant in</t>
+  </si>
+  <si>
+    <t>To 8:52. Long Dispersion</t>
+  </si>
+  <si>
+    <t>To 11:51. Long Dispersion</t>
+  </si>
+  <si>
+    <t>To 13:43. Long Dispersion</t>
+  </si>
+  <si>
+    <t>To 13:38. Long Dispersion</t>
+  </si>
+  <si>
+    <t>To 11:43. Long Dispersion</t>
+  </si>
+  <si>
+    <t>There might be nose whistlers? Closer to midnight in Burst. Also checksurvey</t>
+  </si>
+  <si>
+    <t>Redo? Didn’t see much in burst</t>
+  </si>
+  <si>
+    <t>This was really bad… could you look at this?</t>
+  </si>
+  <si>
+    <t>13:37 to 13:37:10 confusing… look at with George, and add the ones past it to like 13:37:50</t>
+  </si>
+  <si>
+    <t>Burst Mode 2023 11 22 8:24 seems to have a ton, but also a lot of overlap with burst? Check in on again</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -241,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -257,6 +299,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -572,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC498C93-F059-4B72-BF6C-12165486DAC9}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -621,10 +666,10 @@
         <v>35</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -691,7 +736,7 @@
         <v>34</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>34</v>
@@ -811,7 +856,7 @@
         <v>39</v>
       </c>
       <c r="N6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -888,7 +933,7 @@
         <v>34</v>
       </c>
       <c r="N8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -1008,7 +1053,7 @@
         <v>34</v>
       </c>
       <c r="N11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -1131,7 +1176,7 @@
         <v>34</v>
       </c>
       <c r="N14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -1175,7 +1220,7 @@
         <v>34</v>
       </c>
       <c r="N15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -1210,7 +1255,7 @@
         <v>24</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L16" s="4" t="s">
         <v>34</v>
@@ -1219,7 +1264,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>2021</v>
       </c>
@@ -1257,7 +1302,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
         <v>2021</v>
       </c>
@@ -1295,7 +1340,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
@@ -1336,7 +1381,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
@@ -1377,15 +1422,257 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L23" s="3" t="s">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B22" s="1">
+        <v>2019</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1">
+        <v>12</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.52361111111111114</v>
+      </c>
+      <c r="J22" t="s">
         <v>49</v>
       </c>
+      <c r="K22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B23" s="1">
+        <v>2019</v>
+      </c>
+      <c r="C23" s="1">
+        <v>11</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.75486111111111109</v>
+      </c>
+      <c r="J23" t="s">
+        <v>50</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O23" s="3"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B24" s="1">
+        <v>2020</v>
+      </c>
+      <c r="C24" s="1">
+        <v>9</v>
+      </c>
+      <c r="D24" s="1">
+        <v>15</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.8881944444444444</v>
+      </c>
+      <c r="J24" t="s">
+        <v>51</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B25" s="1">
+        <v>2021</v>
+      </c>
+      <c r="C25" s="1">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1">
+        <v>8</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.35694444444444445</v>
+      </c>
+      <c r="J25" t="s">
+        <v>52</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" s="8"/>
+      <c r="B26" s="1">
+        <v>2023</v>
+      </c>
+      <c r="C26" s="1">
+        <v>11</v>
+      </c>
+      <c r="D26" s="1">
+        <v>22</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="J26" t="s">
+        <v>53</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="8"/>
+      <c r="B27" s="1">
+        <v>2023</v>
+      </c>
+      <c r="C27" s="1">
+        <v>11</v>
+      </c>
+      <c r="D27" s="1">
+        <v>22</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.48819444444444443</v>
+      </c>
+      <c r="J27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28" s="8"/>
+      <c r="B28" s="1">
+        <v>2023</v>
+      </c>
+      <c r="C28" s="1">
+        <v>11</v>
+      </c>
+      <c r="D28" s="1">
+        <v>22</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.56874999999999998</v>
+      </c>
+      <c r="J28" t="s">
+        <v>55</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" s="8"/>
+      <c r="B29" s="1">
+        <v>2022</v>
+      </c>
+      <c r="C29" s="1">
+        <v>9</v>
+      </c>
+      <c r="D29" s="1">
+        <v>29</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.56527777777777777</v>
+      </c>
+      <c r="J29" t="s">
+        <v>56</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" s="8"/>
+      <c r="B30" s="1">
+        <v>2022</v>
+      </c>
+      <c r="C30" s="1">
+        <v>8</v>
+      </c>
+      <c r="D30" s="1">
+        <v>17</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0.48749999999999999</v>
+      </c>
+      <c r="J30" t="s">
+        <v>57</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" s="8"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" s="8"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" s="8"/>
+      <c r="N33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" s="8"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" s="8"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="8"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>